<commit_message>
Nombre de los cuadros
</commit_message>
<xml_diff>
--- a/Cuadros.xlsx
+++ b/Cuadros.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescamanging/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescamanging/Documents/GitHub/ProyectoDAW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F626E8-FFFB-0643-ABB5-760025E0DF73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E62630-0AFB-BF4C-9C53-C1E904904305}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12740" yWindow="0" windowWidth="23040" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
   <si>
     <t>KM-00121</t>
   </si>
@@ -129,9 +129,6 @@
     <t>ET-00160</t>
   </si>
   <si>
-    <t>ARBUSTO C/SALIENTES GEOMETRICOS</t>
-  </si>
-  <si>
     <t>ET-00163</t>
   </si>
   <si>
@@ -373,6 +370,12 @@
   </si>
   <si>
     <t>PRECIO</t>
+  </si>
+  <si>
+    <t>ARBUSTO CON SALIENTES GEOMETRICOS</t>
+  </si>
+  <si>
+    <t>BPM-00128</t>
   </si>
 </sst>
 </file>
@@ -692,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -704,16 +707,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -752,16 +755,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
         <v>107</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>108</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>109</v>
-      </c>
-      <c r="D4" t="s">
-        <v>110</v>
       </c>
       <c r="E4">
         <v>1200</v>
@@ -803,7 +806,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -942,7 +945,7 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -956,10 +959,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
@@ -973,16 +976,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17">
         <v>2800</v>
@@ -990,16 +993,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18">
         <v>2800</v>
@@ -1007,16 +1010,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19">
         <v>2800</v>
@@ -1024,16 +1027,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
-        <v>47</v>
-      </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <v>3200</v>
@@ -1041,16 +1044,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>3200</v>
@@ -1058,16 +1061,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>52</v>
       </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22">
         <v>2500</v>
@@ -1075,16 +1078,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>58</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>59</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
       </c>
       <c r="E23">
         <v>1200</v>
@@ -1092,16 +1095,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
       <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
         <v>59</v>
-      </c>
-      <c r="D24" t="s">
-        <v>60</v>
       </c>
       <c r="E24">
         <v>1200</v>
@@ -1109,16 +1112,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
         <v>63</v>
       </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
       <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
         <v>59</v>
-      </c>
-      <c r="D25" t="s">
-        <v>60</v>
       </c>
       <c r="E25">
         <v>1200</v>
@@ -1126,16 +1129,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
         <v>65</v>
       </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
       <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
         <v>59</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
       </c>
       <c r="E26">
         <v>1200</v>
@@ -1143,16 +1146,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="B27" t="s">
-        <v>68</v>
-      </c>
       <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
         <v>59</v>
-      </c>
-      <c r="D27" t="s">
-        <v>60</v>
       </c>
       <c r="E27">
         <v>1200</v>
@@ -1160,16 +1163,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
         <v>69</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>70</v>
       </c>
-      <c r="C28" t="s">
-        <v>71</v>
-      </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28">
         <v>1400</v>
@@ -1177,16 +1180,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
         <v>73</v>
-      </c>
-      <c r="C29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" t="s">
-        <v>74</v>
       </c>
       <c r="E29">
         <v>1400</v>
@@ -1194,16 +1197,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
         <v>75</v>
       </c>
-      <c r="B30" t="s">
-        <v>76</v>
-      </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E30">
         <v>1400</v>
@@ -1211,16 +1214,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
         <v>77</v>
       </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>78</v>
-      </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E31">
         <v>1200</v>
@@ -1228,16 +1231,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
         <v>79</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>80</v>
       </c>
-      <c r="C32" t="s">
-        <v>81</v>
-      </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E32">
         <v>1200</v>
@@ -1245,16 +1248,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
         <v>82</v>
       </c>
-      <c r="B33" t="s">
-        <v>83</v>
-      </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33">
         <v>1200</v>
@@ -1262,16 +1265,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s">
         <v>84</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" t="s">
         <v>85</v>
-      </c>
-      <c r="C34" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" t="s">
-        <v>86</v>
       </c>
       <c r="E34">
         <v>1200</v>
@@ -1279,16 +1282,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
         <v>87</v>
       </c>
-      <c r="B35" t="s">
-        <v>88</v>
-      </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E35">
         <v>1200</v>
@@ -1296,16 +1299,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
         <v>89</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>90</v>
       </c>
-      <c r="C36" t="s">
-        <v>91</v>
-      </c>
       <c r="D36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E36">
         <v>900</v>
@@ -1313,16 +1316,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" t="s">
         <v>92</v>
       </c>
-      <c r="C37" t="s">
-        <v>93</v>
-      </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37">
         <v>1400</v>
@@ -1330,16 +1333,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
         <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E38">
         <v>1400</v>
@@ -1347,16 +1350,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
         <v>95</v>
       </c>
-      <c r="C39" t="s">
-        <v>96</v>
-      </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E39">
         <v>1200</v>
@@ -1364,16 +1367,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40">
         <v>1200</v>
@@ -1381,16 +1384,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" t="s">
         <v>97</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>98</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>99</v>
-      </c>
-      <c r="D41" t="s">
-        <v>100</v>
       </c>
       <c r="E41">
         <v>3200</v>
@@ -1398,16 +1401,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" t="s">
         <v>101</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>102</v>
       </c>
-      <c r="C42" t="s">
-        <v>103</v>
-      </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E42">
         <v>3200</v>
@@ -1415,16 +1418,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
         <v>104</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>105</v>
       </c>
-      <c r="C43" t="s">
-        <v>106</v>
-      </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E43">
         <v>2800</v>

</xml_diff>